<commit_message>
1) Array -> Third Question -> Max SubArray -> Approach1 and Approach2 Implemented 2) Array -> Fourth Question -> ContainsDuplicate -> Approach1  and Approach2 Implemented 3) DSA Sheet Updated
</commit_message>
<xml_diff>
--- a/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PA40084335/Desktop/IMP (Study Material)/DSA Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA818FE-50A6-E24B-A97C-2110F4C1F8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56733D16-9039-2044-969B-5172EEDC4DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="23600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2380" yWindow="500" windowWidth="34880" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA in 2.5 Months" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="705">
   <si>
     <t>DSA by Shradha Didi &amp; Aman Bhaiya</t>
   </si>
@@ -2158,12 +2158,21 @@
 P - PENDING
 C - Completed</t>
   </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Try another optimum/different solution</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2346,7 +2355,21 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2357,7 +2380,7 @@
       <name val="Open Sans"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2414,7 +2437,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -2427,11 +2460,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2543,18 +2578,29 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="11" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="11" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2774,8 +2820,8 @@
   </sheetPr>
   <dimension ref="A1:AA919"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3070,9 +3116,15 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="45"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="47" t="s">
+        <v>702</v>
+      </c>
+      <c r="B10" s="46" t="s">
+        <v>703</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>704</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="45" t="s">
         <v>701</v>
@@ -3139,7 +3191,7 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -3150,9 +3202,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E12" s="46"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -3176,7 +3226,7 @@
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
@@ -3187,9 +3237,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E13" s="46"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -3213,7 +3261,7 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
@@ -3226,9 +3274,7 @@
       <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E14" s="46"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -3263,9 +3309,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E15" s="43"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -3300,9 +3344,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E16" s="43"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -3337,9 +3379,7 @@
         <v>26</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E17" s="43"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -3374,9 +3414,7 @@
         <v>28</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E18" s="43"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -3411,9 +3449,7 @@
         <v>30</v>
       </c>
       <c r="D19" s="13"/>
-      <c r="E19" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E19" s="43"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -3448,9 +3484,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="13"/>
-      <c r="E20" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E20" s="43"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -3485,9 +3519,7 @@
         <v>33</v>
       </c>
       <c r="D21" s="13"/>
-      <c r="E21" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E21" s="43"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -3524,9 +3556,7 @@
       <c r="D22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E22" s="43"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -3561,9 +3591,7 @@
         <v>20</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E23" s="43"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -3598,9 +3626,7 @@
         <v>39</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E24" s="43"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -3635,9 +3661,7 @@
         <v>41</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E25" s="43"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -3672,9 +3696,7 @@
         <v>43</v>
       </c>
       <c r="D26" s="2"/>
-      <c r="E26" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E26" s="43"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -3709,9 +3731,7 @@
         <v>41</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E27" s="43"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -3748,9 +3768,7 @@
       <c r="D28" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E28" s="43"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -3785,9 +3803,7 @@
         <v>49</v>
       </c>
       <c r="D29" s="2"/>
-      <c r="E29" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E29" s="43"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -3822,9 +3838,7 @@
         <v>16</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E30" s="43"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -3859,9 +3873,7 @@
         <v>52</v>
       </c>
       <c r="D31" s="44"/>
-      <c r="E31" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E31" s="43"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -3896,9 +3908,7 @@
         <v>54</v>
       </c>
       <c r="D32" s="2"/>
-      <c r="E32" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E32" s="43"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -3933,9 +3943,7 @@
         <v>56</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E33" s="43"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -3970,9 +3978,7 @@
         <v>54</v>
       </c>
       <c r="D34" s="2"/>
-      <c r="E34" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E34" s="43"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -4007,9 +4013,7 @@
         <v>59</v>
       </c>
       <c r="D35" s="2"/>
-      <c r="E35" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E35" s="43"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -4044,9 +4048,7 @@
         <v>54</v>
       </c>
       <c r="D36" s="2"/>
-      <c r="E36" s="43" t="s">
-        <v>700</v>
-      </c>
+      <c r="E36" s="43"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -32724,7 +32726,9 @@
   </sheetPr>
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
1) Array -> Sixth Question -> Search in Rotated Sorted array -> Approach1 and Approach2 Implemented 3) DSA Sheet Updated
</commit_message>
<xml_diff>
--- a/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PA40084335/Documents/ParryApplications/IntelliJ_Practice/DSASheetPractice/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BB2C85-653D-4B4A-99BB-E8FAC323BCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5790198C-E31A-BB4F-A9E9-92C4A06AB49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="500" windowWidth="34880" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2831,8 +2831,8 @@
   </sheetPr>
   <dimension ref="A1:AB919"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3383,7 +3383,7 @@
         <v>23</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="39"/>
+      <c r="F16" s="42"/>
       <c r="G16">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
1) String -> First Question -> Valid Palindrome -> Approach1 , Approach2 and Approach3 Implemented 3) DSA Sheet Updated
</commit_message>
<xml_diff>
--- a/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PA40084335/Documents/ParryApplications/IntelliJ_Practice/DSASheetPractice/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5790198C-E31A-BB4F-A9E9-92C4A06AB49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDA7505-3902-7944-9CCF-9A8430299D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="500" windowWidth="34880" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2831,8 +2831,8 @@
   </sheetPr>
   <dimension ref="A1:AB919"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3423,7 +3423,7 @@
         <v>26</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="39"/>
+      <c r="F17" s="42"/>
       <c r="G17">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
1) String -> First Question -> Valid Palindrome -> Approach4 Implemented 3) DSA Sheet Updated
</commit_message>
<xml_diff>
--- a/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PA40084335/Documents/ParryApplications/IntelliJ_Practice/DSASheetPractice/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDA7505-3902-7944-9CCF-9A8430299D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181FD13B-0A3C-5947-9774-B1696E96FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="500" windowWidth="34880" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="706">
   <si>
     <t>DSA by Shradha Didi &amp; Aman Bhaiya</t>
   </si>
@@ -2831,8 +2831,8 @@
   </sheetPr>
   <dimension ref="A1:AB919"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4322,9 +4322,7 @@
         <v>65</v>
       </c>
       <c r="E40" s="2"/>
-      <c r="F40" s="39" t="s">
-        <v>700</v>
-      </c>
+      <c r="F40" s="42"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>

</xml_diff>

<commit_message>
1) String -> Second Question -> Valid Anagram -> Approach1 and Approach2 Implemented 3) DSA Sheet Updated
</commit_message>
<xml_diff>
--- a/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PA40084335/Documents/ParryApplications/IntelliJ_Practice/DSASheetPractice/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181FD13B-0A3C-5947-9774-B1696E96FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5FF92A-FE86-694B-9439-1B8E6DCE9F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="500" windowWidth="34880" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2831,8 +2831,8 @@
   </sheetPr>
   <dimension ref="A1:AB919"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4322,7 +4322,7 @@
         <v>65</v>
       </c>
       <c r="E40" s="2"/>
-      <c r="F40" s="42"/>
+      <c r="F40" s="44"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>

</xml_diff>

<commit_message>
1) String -> Third Question -> Valid Parenthesis -> Approach1 and Approach2 Implemented 3) DSA Sheet Updated
</commit_message>
<xml_diff>
--- a/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PA40084335/Documents/ParryApplications/IntelliJ_Practice/DSASheetPractice/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5FF92A-FE86-694B-9439-1B8E6DCE9F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82639A8-5788-D64C-BCB8-E4B70C68707A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="500" windowWidth="34880" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="706">
   <si>
     <t>DSA by Shradha Didi &amp; Aman Bhaiya</t>
   </si>
@@ -2832,7 +2832,7 @@
   <dimension ref="A1:AB919"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4357,9 +4357,7 @@
         <v>67</v>
       </c>
       <c r="E41" s="2"/>
-      <c r="F41" s="39" t="s">
-        <v>700</v>
-      </c>
+      <c r="F41" s="44"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>

</xml_diff>

<commit_message>
1) String -> Fourth Question -> Remove Consecutive Characters -> Approach1 and Approach2 Implemented 3) DSA Sheet Updated
</commit_message>
<xml_diff>
--- a/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PA40084335/Documents/ParryApplications/IntelliJ_Practice/DSASheetPractice/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82639A8-5788-D64C-BCB8-E4B70C68707A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E722477A-DD84-2949-A961-68678C69BE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="500" windowWidth="34880" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="706">
   <si>
     <t>DSA by Shradha Didi &amp; Aman Bhaiya</t>
   </si>
@@ -2831,8 +2831,8 @@
   </sheetPr>
   <dimension ref="A1:AB919"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4312,6 +4312,9 @@
       <c r="AB39" s="2"/>
     </row>
     <row r="40" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1</v>
+      </c>
       <c r="B40" s="5" t="s">
         <v>63</v>
       </c>
@@ -4323,7 +4326,9 @@
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="44"/>
-      <c r="G40" s="2"/>
+      <c r="G40">
+        <v>1</v>
+      </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -4347,6 +4352,9 @@
       <c r="AB40" s="2"/>
     </row>
     <row r="41" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2</v>
+      </c>
       <c r="B41" s="5" t="s">
         <v>63</v>
       </c>
@@ -4358,7 +4366,9 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="44"/>
-      <c r="G41" s="2"/>
+      <c r="G41">
+        <v>2</v>
+      </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -4382,6 +4392,9 @@
       <c r="AB41" s="2"/>
     </row>
     <row r="42" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>3</v>
+      </c>
       <c r="B42" s="5" t="s">
         <v>63</v>
       </c>
@@ -4394,10 +4407,10 @@
       <c r="E42" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F42" s="39" t="s">
-        <v>700</v>
-      </c>
-      <c r="G42" s="2"/>
+      <c r="F42" s="44"/>
+      <c r="G42">
+        <v>3</v>
+      </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -4421,6 +4434,9 @@
       <c r="AB42" s="2"/>
     </row>
     <row r="43" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>4</v>
+      </c>
       <c r="B43" s="5" t="s">
         <v>63</v>
       </c>
@@ -4434,7 +4450,9 @@
       <c r="F43" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G43" s="2"/>
+      <c r="G43">
+        <v>4</v>
+      </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -4458,6 +4476,9 @@
       <c r="AB43" s="2"/>
     </row>
     <row r="44" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>5</v>
+      </c>
       <c r="B44" s="5" t="s">
         <v>63</v>
       </c>
@@ -4471,7 +4492,9 @@
       <c r="F44" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G44" s="2"/>
+      <c r="G44">
+        <v>5</v>
+      </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -4495,6 +4518,9 @@
       <c r="AB44" s="2"/>
     </row>
     <row r="45" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>6</v>
+      </c>
       <c r="B45" s="5" t="s">
         <v>63</v>
       </c>
@@ -4508,7 +4534,9 @@
       <c r="F45" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G45" s="2"/>
+      <c r="G45">
+        <v>6</v>
+      </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -4532,6 +4560,9 @@
       <c r="AB45" s="2"/>
     </row>
     <row r="46" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>7</v>
+      </c>
       <c r="B46" s="5" t="s">
         <v>63</v>
       </c>
@@ -4545,7 +4576,9 @@
       <c r="F46" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G46" s="2"/>
+      <c r="G46">
+        <v>7</v>
+      </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -4569,6 +4602,9 @@
       <c r="AB46" s="2"/>
     </row>
     <row r="47" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>8</v>
+      </c>
       <c r="B47" s="8" t="s">
         <v>63</v>
       </c>
@@ -4582,7 +4618,9 @@
       <c r="F47" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G47" s="2"/>
+      <c r="G47">
+        <v>8</v>
+      </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -4606,6 +4644,9 @@
       <c r="AB47" s="2"/>
     </row>
     <row r="48" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>9</v>
+      </c>
       <c r="B48" s="8" t="s">
         <v>63</v>
       </c>
@@ -4619,7 +4660,9 @@
       <c r="F48" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G48" s="2"/>
+      <c r="G48">
+        <v>9</v>
+      </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -4642,7 +4685,10 @@
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>10</v>
+      </c>
       <c r="B49" s="8" t="s">
         <v>63</v>
       </c>
@@ -4656,7 +4702,9 @@
       <c r="F49" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G49" s="2"/>
+      <c r="G49">
+        <v>10</v>
+      </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -4679,7 +4727,10 @@
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>11</v>
+      </c>
       <c r="B50" s="8" t="s">
         <v>63</v>
       </c>
@@ -4693,7 +4744,9 @@
       <c r="F50" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G50" s="2"/>
+      <c r="G50">
+        <v>11</v>
+      </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -4716,7 +4769,10 @@
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>12</v>
+      </c>
       <c r="B51" s="8" t="s">
         <v>63</v>
       </c>
@@ -4730,7 +4786,9 @@
       <c r="F51" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G51" s="2"/>
+      <c r="G51">
+        <v>12</v>
+      </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -4753,7 +4811,10 @@
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>13</v>
+      </c>
       <c r="B52" s="8" t="s">
         <v>63</v>
       </c>
@@ -4767,7 +4828,9 @@
       <c r="F52" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G52" s="2"/>
+      <c r="G52">
+        <v>13</v>
+      </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -4790,7 +4853,10 @@
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>14</v>
+      </c>
       <c r="B53" s="8" t="s">
         <v>63</v>
       </c>
@@ -4804,7 +4870,9 @@
       <c r="F53" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G53" s="2"/>
+      <c r="G53">
+        <v>14</v>
+      </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -4827,7 +4895,10 @@
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>15</v>
+      </c>
       <c r="B54" s="8" t="s">
         <v>63</v>
       </c>
@@ -4841,7 +4912,9 @@
       <c r="F54" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G54" s="2"/>
+      <c r="G54">
+        <v>15</v>
+      </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -4864,7 +4937,10 @@
       <c r="AA54" s="2"/>
       <c r="AB54" s="2"/>
     </row>
-    <row r="55" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>16</v>
+      </c>
       <c r="B55" s="8" t="s">
         <v>63</v>
       </c>
@@ -4878,7 +4954,9 @@
       <c r="F55" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G55" s="2"/>
+      <c r="G55">
+        <v>16</v>
+      </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -4901,7 +4979,10 @@
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
     </row>
-    <row r="56" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>17</v>
+      </c>
       <c r="B56" s="8" t="s">
         <v>63</v>
       </c>
@@ -4915,7 +4996,9 @@
       <c r="F56" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G56" s="2"/>
+      <c r="G56">
+        <v>17</v>
+      </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -4938,7 +5021,10 @@
       <c r="AA56" s="2"/>
       <c r="AB56" s="2"/>
     </row>
-    <row r="57" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>18</v>
+      </c>
       <c r="B57" s="8" t="s">
         <v>63</v>
       </c>
@@ -4952,7 +5038,9 @@
       <c r="F57" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G57" s="2"/>
+      <c r="G57">
+        <v>18</v>
+      </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
@@ -4975,7 +5063,10 @@
       <c r="AA57" s="2"/>
       <c r="AB57" s="2"/>
     </row>
-    <row r="58" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>19</v>
+      </c>
       <c r="B58" s="8" t="s">
         <v>63</v>
       </c>
@@ -4989,7 +5080,9 @@
       <c r="F58" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G58" s="2"/>
+      <c r="G58">
+        <v>19</v>
+      </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
@@ -5012,7 +5105,10 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>20</v>
+      </c>
       <c r="B59" s="9" t="s">
         <v>63</v>
       </c>
@@ -5026,7 +5122,9 @@
       <c r="F59" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G59" s="2"/>
+      <c r="G59">
+        <v>20</v>
+      </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
@@ -5049,7 +5147,10 @@
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
     </row>
-    <row r="60" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>21</v>
+      </c>
       <c r="B60" s="9" t="s">
         <v>63</v>
       </c>
@@ -5063,7 +5164,9 @@
       <c r="F60" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G60" s="2"/>
+      <c r="G60">
+        <v>21</v>
+      </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
@@ -5086,7 +5189,10 @@
       <c r="AA60" s="2"/>
       <c r="AB60" s="2"/>
     </row>
-    <row r="61" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>22</v>
+      </c>
       <c r="B61" s="9" t="s">
         <v>63</v>
       </c>
@@ -5102,7 +5208,9 @@
       <c r="F61" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G61" s="2"/>
+      <c r="G61">
+        <v>22</v>
+      </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -5125,7 +5233,7 @@
       <c r="AA61" s="2"/>
       <c r="AB61" s="2"/>
     </row>
-    <row r="62" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="B62" s="16"/>
       <c r="C62" s="17"/>
       <c r="D62" s="18"/>
@@ -5133,7 +5241,9 @@
       <c r="F62" s="39" t="s">
         <v>700</v>
       </c>
-      <c r="G62" s="2"/>
+      <c r="G62">
+        <v>23</v>
+      </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
@@ -5156,7 +5266,7 @@
       <c r="AA62" s="2"/>
       <c r="AB62" s="2"/>
     </row>
-    <row r="63" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="B63" s="16"/>
       <c r="C63" s="17"/>
       <c r="D63" s="18"/>
@@ -5185,7 +5295,7 @@
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
     </row>
-    <row r="64" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="B64" s="8" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
1) String -> Fifth Question -> LongestCommonPrefix -> Approach1 3) DSA Sheet Updated
</commit_message>
<xml_diff>
--- a/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PA40084335/Documents/ParryApplications/IntelliJ_Practice/DSASheetPractice/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E722477A-DD84-2949-A961-68678C69BE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38198A4C-C418-9542-B2F4-F5F8A88F0CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="500" windowWidth="34880" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="706">
   <si>
     <t>DSA by Shradha Didi &amp; Aman Bhaiya</t>
   </si>
@@ -2832,7 +2832,7 @@
   <dimension ref="A1:AB919"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4447,9 +4447,7 @@
         <v>71</v>
       </c>
       <c r="E43" s="2"/>
-      <c r="F43" s="39" t="s">
-        <v>700</v>
-      </c>
+      <c r="F43" s="44"/>
       <c r="G43">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
1) String -> Sixth Question -> SentenceIntoEquivalentSeq -> Approach1 2) String -> Seventh Question -> DuplicateCharsFromString -> Approach1 3) DSA Sheet Updated 4) TimeComplexity Calculator Added.
</commit_message>
<xml_diff>
--- a/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/out/production/DSASheetPractice/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PA40084335/Documents/ParryApplications/IntelliJ_Practice/DSASheetPractice/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PA40084335/Documents/ParryApplications/FullStack Roadmap Practice/Backend (Java &amp; Spring)/DSASheetPractice/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38198A4C-C418-9542-B2F4-F5F8A88F0CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A963B41-0BAE-284A-BF42-EF95E0AC3281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="500" windowWidth="34880" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2380" yWindow="500" windowWidth="35820" windowHeight="21880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA in 2.5 Months" sheetId="1" r:id="rId1"/>
@@ -24,16 +24,16 @@
   </definedNames>
   <calcPr calcId="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{A2FC19DB-909B-4030-B2C2-F31C9B72C5DC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{7F344D43-7868-40B3-9097-AEF176B3194E}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{506D7840-D91F-4215-91FA-E391829E2303}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{FA99C533-7283-4917-B47A-8ACF4F782944}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{506D7840-D91F-4215-91FA-E391829E2303}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{7F344D43-7868-40B3-9097-AEF176B3194E}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A2FC19DB-909B-4030-B2C2-F31C9B72C5DC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="706">
   <si>
     <t>DSA by Shradha Didi &amp; Aman Bhaiya</t>
   </si>
@@ -2596,6 +2596,7 @@
     <xf numFmtId="0" fontId="32" fillId="12" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2606,7 +2607,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2831,8 +2831,8 @@
   </sheetPr>
   <dimension ref="A1:AB919"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2846,11 +2846,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="25" x14ac:dyDescent="0.2">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -2877,11 +2877,11 @@
       <c r="AB1" s="2"/>
     </row>
     <row r="2" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -2906,9 +2906,9 @@
       <c r="AB2" s="2"/>
     </row>
     <row r="3" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2937,9 +2937,9 @@
       <c r="AB3" s="2"/>
     </row>
     <row r="4" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -3036,7 +3036,7 @@
       <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="49" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="2"/>
@@ -3071,7 +3071,7 @@
       <c r="C8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="46"/>
+      <c r="D8" s="47"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3164,7 +3164,7 @@
       <c r="AB10" s="2"/>
     </row>
     <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="45" t="s">
         <v>705</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -3182,7 +3182,7 @@
       <c r="F11" s="11" t="s">
         <v>699</v>
       </c>
-      <c r="G11" s="49" t="s">
+      <c r="G11" s="45" t="s">
         <v>705</v>
       </c>
       <c r="H11" s="2"/>
@@ -4487,9 +4487,7 @@
         <v>73</v>
       </c>
       <c r="E44" s="2"/>
-      <c r="F44" s="39" t="s">
-        <v>700</v>
-      </c>
+      <c r="F44" s="44"/>
       <c r="G44">
         <v>5</v>
       </c>
@@ -4529,9 +4527,7 @@
         <v>75</v>
       </c>
       <c r="E45" s="2"/>
-      <c r="F45" s="39" t="s">
-        <v>700</v>
-      </c>
+      <c r="F45" s="44"/>
       <c r="G45">
         <v>6</v>
       </c>
@@ -32562,21 +32558,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{A2FC19DB-909B-4030-B2C2-F31C9B72C5DC}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{506D7840-D91F-4215-91FA-E391829E2303}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{C8330CEA-88E9-DC44-9127-9D9D9122D8E3}"/>
+      <autoFilter ref="A11:C37" xr:uid="{839C3AE7-A9B8-A24A-B8D1-BAB623BD2336}"/>
+    </customSheetView>
+    <customSheetView guid="{7F344D43-7868-40B3-9097-AEF176B3194E}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{A190677E-EE76-8E4A-BD83-C925B2A2F663}"/>
     </customSheetView>
     <customSheetView guid="{FA99C533-7283-4917-B47A-8ACF4F782944}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{301FAC8B-8A93-094C-9EC2-1CBCD33D2136}"/>
+      <autoFilter ref="A11:D37" xr:uid="{C86C859B-A666-FC49-8128-AB9EE3631BDE}"/>
     </customSheetView>
-    <customSheetView guid="{7F344D43-7868-40B3-9097-AEF176B3194E}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{A2FC19DB-909B-4030-B2C2-F31C9B72C5DC}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{AD4687E1-6470-964E-82BF-38802464F5EC}"/>
-    </customSheetView>
-    <customSheetView guid="{506D7840-D91F-4215-91FA-E391829E2303}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{74073A75-8FFD-F74E-AD56-9211AAE99416}"/>
+      <autoFilter ref="A293:C332" xr:uid="{ECDD3328-3DA3-C84A-AC27-4C4F03768CB0}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="3">
@@ -32988,28 +32984,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="46"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>

</xml_diff>